<commit_message>
Updading Fragility Curves Gen Tech
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/EIAData/NC Energy Average Data Statistics EIA.xlsx
+++ b/CreateDB_NC/InputData/EIAData/NC Energy Average Data Statistics EIA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\EIAData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761FE765-F3E7-4D56-A561-4E477B4E7A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E683023-7C42-4957-A43A-462EF0513AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Summary" sheetId="1" r:id="rId1"/>
@@ -1698,6 +1698,7 @@
     <xf numFmtId="165" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1719,7 +1720,6 @@
     <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2059,18 +2059,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2293,11 +2293,11 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2334,46 +2334,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="38" t="s">
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="H3" s="40"/>
+      <c r="H3" s="41"/>
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2611,17 +2611,17 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2643,9 +2643,9 @@
   </sheetPr>
   <dimension ref="A1:AG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B33" sqref="B33:K33"/>
+      <selection pane="topRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2656,115 +2656,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
     </row>
     <row r="2" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
     </row>
     <row r="3" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
     </row>
     <row r="4" spans="1:33" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -5595,83 +5595,83 @@
       </c>
     </row>
     <row r="32" spans="1:33" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="36"/>
-      <c r="U32" s="36"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="36"/>
-      <c r="AA32" s="36"/>
-      <c r="AB32" s="36"/>
-      <c r="AC32" s="36"/>
-      <c r="AD32" s="36"/>
-      <c r="AE32" s="36"/>
-      <c r="AF32" s="36"/>
-      <c r="AG32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="37"/>
+      <c r="U32" s="37"/>
+      <c r="V32" s="37"/>
+      <c r="W32" s="37"/>
+      <c r="X32" s="37"/>
+      <c r="Y32" s="37"/>
+      <c r="Z32" s="37"/>
+      <c r="AA32" s="37"/>
+      <c r="AB32" s="37"/>
+      <c r="AC32" s="37"/>
+      <c r="AD32" s="37"/>
+      <c r="AE32" s="37"/>
+      <c r="AF32" s="37"/>
+      <c r="AG32" s="37"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="B33" s="42">
+      <c r="B33" s="35">
         <f>B26/(B29-B24)*100</f>
         <v>4.4660141183523638</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="35">
         <f t="shared" ref="C33:K33" si="0">C26/(C29-C24)*100</f>
         <v>5.2831235455010592</v>
       </c>
-      <c r="D33" s="42">
+      <c r="D33" s="35">
         <f t="shared" si="0"/>
         <v>5.1313371830231524</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="35">
         <f t="shared" si="0"/>
         <v>4.8758001052524333</v>
       </c>
-      <c r="F33" s="42">
+      <c r="F33" s="35">
         <f t="shared" si="0"/>
         <v>5.125315128593515</v>
       </c>
-      <c r="G33" s="42">
+      <c r="G33" s="35">
         <f t="shared" si="0"/>
         <v>4.9024148417244646</v>
       </c>
-      <c r="H33" s="42">
+      <c r="H33" s="35">
         <f t="shared" si="0"/>
         <v>4.6820269925066622</v>
       </c>
-      <c r="I33" s="42">
+      <c r="I33" s="35">
         <f t="shared" si="0"/>
         <v>4.8891980519903466</v>
       </c>
-      <c r="J33" s="42">
+      <c r="J33" s="35">
         <f t="shared" si="0"/>
         <v>5.0261410187495654</v>
       </c>
-      <c r="K33" s="42">
+      <c r="K33" s="35">
         <f t="shared" si="0"/>
         <v>5.0551916590894344</v>
       </c>
@@ -5710,38 +5710,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
     </row>
     <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
     </row>
     <row r="3" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -8942,21 +8942,21 @@
       </c>
     </row>
     <row r="81" spans="1:13" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="36" t="s">
+      <c r="A81" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B81" s="36"/>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="36"/>
-      <c r="H81" s="36"/>
-      <c r="I81" s="36"/>
-      <c r="J81" s="36"/>
-      <c r="K81" s="36"/>
-      <c r="L81" s="36"/>
-      <c r="M81" s="36"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="37"/>
+      <c r="G81" s="37"/>
+      <c r="H81" s="37"/>
+      <c r="I81" s="37"/>
+      <c r="J81" s="37"/>
+      <c r="K81" s="37"/>
+      <c r="L81" s="37"/>
+      <c r="M81" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8978,7 +8978,7 @@
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8989,44 +8989,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
     </row>
     <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -10079,24 +10079,24 @@
       </c>
     </row>
     <row r="24" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10131,32 +10131,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -11535,18 +11535,18 @@
       </c>
     </row>
     <row r="46" spans="1:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -11566,11 +11566,11 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11582,44 +11582,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
     </row>
     <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -11672,24 +11672,24 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -12342,24 +12342,24 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -12512,24 +12512,24 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -12567,44 +12567,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
     </row>
     <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -12657,24 +12657,24 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="42" t="s">
         <v>244</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -13327,24 +13327,24 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -13497,24 +13497,24 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -13549,37 +13549,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -14985,15 +14985,15 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="36" t="s">
+      <c r="A65" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -15027,32 +15027,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -16047,18 +16047,18 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="37" t="s">
         <v>283</v>
       </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -16078,7 +16078,9 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16091,22 +16093,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -16296,13 +16298,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -16335,22 +16337,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -16540,13 +16542,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -16578,40 +16580,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -16822,16 +16824,16 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -16868,127 +16870,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
     </row>
     <row r="2" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="35"/>
-      <c r="AI2" s="35"/>
-      <c r="AJ2" s="35"/>
-      <c r="AK2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
     </row>
     <row r="3" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="38"/>
+      <c r="AI3" s="38"/>
+      <c r="AJ3" s="38"/>
+      <c r="AK3" s="38"/>
     </row>
     <row r="4" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -23206,45 +23208,45 @@
       </c>
     </row>
     <row r="59" spans="1:37" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="36"/>
-      <c r="J59" s="36"/>
-      <c r="K59" s="36"/>
-      <c r="L59" s="36"/>
-      <c r="M59" s="36"/>
-      <c r="N59" s="36"/>
-      <c r="O59" s="36"/>
-      <c r="P59" s="36"/>
-      <c r="Q59" s="36"/>
-      <c r="R59" s="36"/>
-      <c r="S59" s="36"/>
-      <c r="T59" s="36"/>
-      <c r="U59" s="36"/>
-      <c r="V59" s="36"/>
-      <c r="W59" s="36"/>
-      <c r="X59" s="36"/>
-      <c r="Y59" s="36"/>
-      <c r="Z59" s="36"/>
-      <c r="AA59" s="36"/>
-      <c r="AB59" s="36"/>
-      <c r="AC59" s="36"/>
-      <c r="AD59" s="36"/>
-      <c r="AE59" s="36"/>
-      <c r="AF59" s="36"/>
-      <c r="AG59" s="36"/>
-      <c r="AH59" s="36"/>
-      <c r="AI59" s="36"/>
-      <c r="AJ59" s="36"/>
-      <c r="AK59" s="36"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="37"/>
+      <c r="O59" s="37"/>
+      <c r="P59" s="37"/>
+      <c r="Q59" s="37"/>
+      <c r="R59" s="37"/>
+      <c r="S59" s="37"/>
+      <c r="T59" s="37"/>
+      <c r="U59" s="37"/>
+      <c r="V59" s="37"/>
+      <c r="W59" s="37"/>
+      <c r="X59" s="37"/>
+      <c r="Y59" s="37"/>
+      <c r="Z59" s="37"/>
+      <c r="AA59" s="37"/>
+      <c r="AB59" s="37"/>
+      <c r="AC59" s="37"/>
+      <c r="AD59" s="37"/>
+      <c r="AE59" s="37"/>
+      <c r="AF59" s="37"/>
+      <c r="AG59" s="37"/>
+      <c r="AH59" s="37"/>
+      <c r="AI59" s="37"/>
+      <c r="AJ59" s="37"/>
+      <c r="AK59" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -23280,127 +23282,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
     </row>
     <row r="2" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="35"/>
-      <c r="AI2" s="35"/>
-      <c r="AJ2" s="35"/>
-      <c r="AK2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
     </row>
     <row r="3" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="38"/>
+      <c r="AI3" s="38"/>
+      <c r="AJ3" s="38"/>
+      <c r="AK3" s="38"/>
     </row>
     <row r="4" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -30635,45 +30637,45 @@
       </c>
     </row>
     <row r="68" spans="1:37" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="36" t="s">
+      <c r="A68" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="36"/>
-      <c r="J68" s="36"/>
-      <c r="K68" s="36"/>
-      <c r="L68" s="36"/>
-      <c r="M68" s="36"/>
-      <c r="N68" s="36"/>
-      <c r="O68" s="36"/>
-      <c r="P68" s="36"/>
-      <c r="Q68" s="36"/>
-      <c r="R68" s="36"/>
-      <c r="S68" s="36"/>
-      <c r="T68" s="36"/>
-      <c r="U68" s="36"/>
-      <c r="V68" s="36"/>
-      <c r="W68" s="36"/>
-      <c r="X68" s="36"/>
-      <c r="Y68" s="36"/>
-      <c r="Z68" s="36"/>
-      <c r="AA68" s="36"/>
-      <c r="AB68" s="36"/>
-      <c r="AC68" s="36"/>
-      <c r="AD68" s="36"/>
-      <c r="AE68" s="36"/>
-      <c r="AF68" s="36"/>
-      <c r="AG68" s="36"/>
-      <c r="AH68" s="36"/>
-      <c r="AI68" s="36"/>
-      <c r="AJ68" s="36"/>
-      <c r="AK68" s="36"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="37"/>
+      <c r="O68" s="37"/>
+      <c r="P68" s="37"/>
+      <c r="Q68" s="37"/>
+      <c r="R68" s="37"/>
+      <c r="S68" s="37"/>
+      <c r="T68" s="37"/>
+      <c r="U68" s="37"/>
+      <c r="V68" s="37"/>
+      <c r="W68" s="37"/>
+      <c r="X68" s="37"/>
+      <c r="Y68" s="37"/>
+      <c r="Z68" s="37"/>
+      <c r="AA68" s="37"/>
+      <c r="AB68" s="37"/>
+      <c r="AC68" s="37"/>
+      <c r="AD68" s="37"/>
+      <c r="AE68" s="37"/>
+      <c r="AF68" s="37"/>
+      <c r="AG68" s="37"/>
+      <c r="AH68" s="37"/>
+      <c r="AI68" s="37"/>
+      <c r="AJ68" s="37"/>
+      <c r="AK68" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -30707,78 +30709,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
     </row>
     <row r="2" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
     </row>
     <row r="3" spans="1:33" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -31690,41 +31692,41 @@
       </c>
     </row>
     <row r="12" spans="1:33" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="36"/>
-      <c r="AA12" s="36"/>
-      <c r="AB12" s="36"/>
-      <c r="AC12" s="36"/>
-      <c r="AD12" s="36"/>
-      <c r="AE12" s="36"/>
-      <c r="AF12" s="36"/>
-      <c r="AG12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+      <c r="Z12" s="37"/>
+      <c r="AA12" s="37"/>
+      <c r="AB12" s="37"/>
+      <c r="AC12" s="37"/>
+      <c r="AD12" s="37"/>
+      <c r="AE12" s="37"/>
+      <c r="AF12" s="37"/>
+      <c r="AG12" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -31757,78 +31759,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
     </row>
     <row r="2" spans="1:33" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
     </row>
     <row r="3" spans="1:33" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -34154,41 +34156,41 @@
       </c>
     </row>
     <row r="26" spans="1:33" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="36"/>
-      <c r="R26" s="36"/>
-      <c r="S26" s="36"/>
-      <c r="T26" s="36"/>
-      <c r="U26" s="36"/>
-      <c r="V26" s="36"/>
-      <c r="W26" s="36"/>
-      <c r="X26" s="36"/>
-      <c r="Y26" s="36"/>
-      <c r="Z26" s="36"/>
-      <c r="AA26" s="36"/>
-      <c r="AB26" s="36"/>
-      <c r="AC26" s="36"/>
-      <c r="AD26" s="36"/>
-      <c r="AE26" s="36"/>
-      <c r="AF26" s="36"/>
-      <c r="AG26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="37"/>
+      <c r="W26" s="37"/>
+      <c r="X26" s="37"/>
+      <c r="Y26" s="37"/>
+      <c r="Z26" s="37"/>
+      <c r="AA26" s="37"/>
+      <c r="AB26" s="37"/>
+      <c r="AC26" s="37"/>
+      <c r="AD26" s="37"/>
+      <c r="AE26" s="37"/>
+      <c r="AF26" s="37"/>
+      <c r="AG26" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -34222,86 +34224,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
     </row>
     <row r="2" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="35"/>
-      <c r="AI2" s="35"/>
-      <c r="AJ2" s="35"/>
-      <c r="AK2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
     </row>
     <row r="3" spans="1:37" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -37581,45 +37583,45 @@
       </c>
     </row>
     <row r="32" spans="1:37" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="36"/>
-      <c r="U32" s="36"/>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="36"/>
-      <c r="AA32" s="36"/>
-      <c r="AB32" s="36"/>
-      <c r="AC32" s="36"/>
-      <c r="AD32" s="36"/>
-      <c r="AE32" s="36"/>
-      <c r="AF32" s="36"/>
-      <c r="AG32" s="36"/>
-      <c r="AH32" s="36"/>
-      <c r="AI32" s="36"/>
-      <c r="AJ32" s="36"/>
-      <c r="AK32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="37"/>
+      <c r="U32" s="37"/>
+      <c r="V32" s="37"/>
+      <c r="W32" s="37"/>
+      <c r="X32" s="37"/>
+      <c r="Y32" s="37"/>
+      <c r="Z32" s="37"/>
+      <c r="AA32" s="37"/>
+      <c r="AB32" s="37"/>
+      <c r="AC32" s="37"/>
+      <c r="AD32" s="37"/>
+      <c r="AE32" s="37"/>
+      <c r="AF32" s="37"/>
+      <c r="AG32" s="37"/>
+      <c r="AH32" s="37"/>
+      <c r="AI32" s="37"/>
+      <c r="AJ32" s="37"/>
+      <c r="AK32" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>